<commit_message>
gain de pièces lors d'une victoire
</commit_message>
<xml_diff>
--- a/Journaux_de_travail/Antoine.xlsx
+++ b/Journaux_de_travail/Antoine.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Léger refactoring, ajout de la fonction de recherche du meilleur mot</t>
   </si>
   <si>
-    <t xml:space="preserve">Discussions de groupe, wordanalyzer</t>
+    <t xml:space="preserve">Discussions de groupe, travail sur wordanalyzer</t>
   </si>
   <si>
     <t xml:space="preserve">Relecture du code</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">Implémentation du peek et hint (côté serveur)</t>
   </si>
   <si>
-    <t xml:space="preserve">Endpoint powers complètement implémenté</t>
+    <t xml:space="preserve">Endpoint powers corrigé et opérationel</t>
   </si>
   <si>
     <t xml:space="preserve">Bug fixes, aide à l’implémentation de l’UI</t>
@@ -354,7 +354,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -484,7 +484,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,7 +539,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="8" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,7 +673,7 @@
       </c>
       <c r="C32" s="10" t="n">
         <f aca="false">SUM(C5:C31)</f>
-        <v>78</v>
+        <v>79.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>